<commit_message>
Connect CI db, migrated, populated, apply settings for heroku
</commit_message>
<xml_diff>
--- a/data/products_impex_2.xlsx
+++ b/data/products_impex_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielkraig/Developer/codeinstitute/project-5/goodwill/carols-whimsy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CE2A3BE-55AA-B84A-B7B8-815358158240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C55D0F0-3AD2-E148-B4D7-E9F679316669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{201FFCEC-E124-2B47-9B84-C6699FAD0420}"/>
+    <workbookView xWindow="-1560" yWindow="2120" windowWidth="27640" windowHeight="16940" xr2:uid="{201FFCEC-E124-2B47-9B84-C6699FAD0420}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>YA92229</t>
   </si>
   <si>
-    <t>X071.jpg</t>
-  </si>
-  <si>
     <t>20/16/9CM</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>sku</t>
+  </si>
+  <si>
+    <t>noimage</t>
   </si>
 </sst>
 </file>
@@ -741,7 +741,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -749,58 +749,58 @@
     <row r="1" spans="1:15" s="1" customFormat="1" ht="112.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10"/>
       <c r="B1" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -823,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>